<commit_message>
fixed optimal path for map1
</commit_message>
<xml_diff>
--- a/MapDesigns.xlsx
+++ b/MapDesigns.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desme\LocalDocument\Repo\Reinforcement-Learning-Malmo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DesmenH_RedSpecter\Source\Repos\Reinforcement-Learning-Malmo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B029899-A42A-4E30-BE87-9B760ADAEFC5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4254681E-895E-46A6-BE5C-C2C0D479D6F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{FDBFA2F1-4C98-476F-A615-69E8EC84A2D0}"/>
+    <workbookView xWindow="9705" yWindow="2325" windowWidth="21375" windowHeight="15780" xr2:uid="{FDBFA2F1-4C98-476F-A615-69E8EC84A2D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="6">
   <si>
     <t>Map 1</t>
   </si>
@@ -484,16 +484,16 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="71" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="11" width="14.6328125" customWidth="1"/>
-    <col min="12" max="34" width="15.1796875" customWidth="1"/>
+    <col min="1" max="11" width="14.5703125" customWidth="1"/>
+    <col min="12" max="34" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,7 +504,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="1.2">
+    <row r="2" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -536,8 +536,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="1.2">
-      <c r="B3" s="4"/>
+    <row r="3" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -559,8 +561,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="1.2">
-      <c r="B4" s="3"/>
+    <row r="4" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -578,8 +582,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="1.2">
-      <c r="B5" s="3"/>
+    <row r="5" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -597,11 +603,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="1.2">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+    <row r="6" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="F6" s="6" t="s">
         <v>1</v>
       </c>
@@ -616,7 +630,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="1.2">
+    <row r="7" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3" t="s">
@@ -628,7 +642,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="1.2">
+    <row r="8" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="I8" s="3"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5" t="s">
@@ -640,29 +654,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="1.2">
+    <row r="9" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" ht="72" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="18" ht="72" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="19" ht="72" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="20" ht="72" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="21" ht="72" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="22" ht="72" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="23" ht="72" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="24" ht="72" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="25" ht="72" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>